<commit_message>
buggy. working on inventory recalculation tests.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/material_expense_cancel_test_cases.xlsx
+++ b/soberano/test_cases/material_expense_cancel_test_cases.xlsx
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes \ Field</t>
-  </si>
-  <si>
     <t xml:space="preserve">User18 is NOT allowed to cancel a material expense. User 18 is salesclerk. It has no rights to retrieve expenses.</t>
   </si>
   <si>
@@ -37,10 +34,34 @@
     <t xml:space="preserve">User14 is NOT allowed to cancel a material expense</t>
   </si>
   <si>
-    <t xml:space="preserve">User1 allowed to cancel a material expense</t>
+    <t xml:space="preserve">User1 allowed to cancel a material expense. material_expense_cancelation_log_test_case_22_state_3_mm6.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">check not canceled expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User1 allowed to cancel a material expense. material_expense_cancelation_log_test_case_27_state_5_mm7.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User1 allowed to cancel a material expense. material_expense_cancelation_log_test_case_29_state_6_mm2.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test class OO18_StockTest_check_following_material_expense_cancelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check global stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check stock stored in warehouse mw10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check stock stored in warehouse mw9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check stock stored in warehouse mw8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check stock stored in warehouse mw6</t>
   </si>
 </sst>
 </file>
@@ -161,10 +182,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -192,9 +213,6 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="AMF1" s="1"/>
@@ -208,7 +226,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,7 +234,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -224,7 +242,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,7 +250,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,7 +258,84 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>